<commit_message>
update mst item data
</commit_message>
<xml_diff>
--- a/Ocean/DB_Design OA.xlsx
+++ b/Ocean/DB_Design OA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/my_app/Ocean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36BF04A-D68F-864A-876B-68946E07B7E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DB106D-DD0F-ED4E-B354-D3A73AA78533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="2220" windowWidth="30720" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1100" windowWidth="30720" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OA" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="107">
   <si>
     <t>DB design</t>
   </si>
@@ -311,9 +311,6 @@
     <t>fk_oa_group_id</t>
   </si>
   <si>
-    <t>lg_oa_history</t>
-  </si>
-  <si>
     <t>เก็บประวัติการแก้ไข OA</t>
   </si>
   <si>
@@ -338,19 +335,10 @@
     <t>กลุ่มความรู้ของ OA</t>
   </si>
   <si>
-    <t>REFERENCES ms_oa_group(fk_oa_group_id)</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
     <t>n: normal, p: ปักหมุด</t>
-  </si>
-  <si>
-    <t>REFERENCES tx_oa_data(pk_id)</t>
-  </si>
-  <si>
-    <t>REFERENCES tx_oa_data(id)</t>
   </si>
   <si>
     <t>หัวข้อ</t>
@@ -400,6 +388,51 @@
       </rPr>
       <t>Activity</t>
     </r>
+  </si>
+  <si>
+    <t>lg_oa_data</t>
+  </si>
+  <si>
+    <t>lg_oa_group</t>
+  </si>
+  <si>
+    <t>เก็บ log group ต่าง ๆ ของ oa</t>
+  </si>
+  <si>
+    <t>lg_oa_group_id</t>
+  </si>
+  <si>
+    <t>REFERENCES ms_oa_group(oa_group_id)</t>
+  </si>
+  <si>
+    <t>REFERENCES tx_oa_data(oa_data_id)</t>
+  </si>
+  <si>
+    <t>lg_oa_upload</t>
+  </si>
+  <si>
+    <t>เก็บ log ว่ามีupload file อะไรบ้าง</t>
+  </si>
+  <si>
+    <t>REFERENCES tx_oa_upload(oa_upload_id)</t>
+  </si>
+  <si>
+    <t>fk_oa_upload_id</t>
+  </si>
+  <si>
+    <t>lg_oa_upload_id</t>
+  </si>
+  <si>
+    <t>lg_oa_position</t>
+  </si>
+  <si>
+    <t>เก็บ log ว่าตำแหน่งไหนเห็น OA นี้บ้าง</t>
+  </si>
+  <si>
+    <t>fk_oa_position_id</t>
+  </si>
+  <si>
+    <t>REFERENCES tx_oa_position(oa_position_id)</t>
   </si>
 </sst>
 </file>
@@ -851,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1009,22 +1042,26 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1033,19 +1070,21 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1428,11 +1467,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T1016"/>
+  <dimension ref="A1:T1044"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D69" sqref="D69"/>
+      <pane ySplit="2" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -1453,23 +1492,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="82" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
       <c r="N1" s="2"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -1529,18 +1568,18 @@
       <c r="T2" s="11"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="79"/>
+      <c r="F3" s="81"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14"/>
       <c r="I3" s="15"/>
@@ -1557,18 +1596,18 @@
       <c r="T3" s="18"/>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="80"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="80"/>
+      <c r="E4" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="82"/>
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22"/>
@@ -1632,10 +1671,10 @@
         <v>20</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="G6" s="38"/>
       <c r="H6" s="39"/>
@@ -1664,7 +1703,7 @@
         <v>27</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="37"/>
@@ -1721,10 +1760,10 @@
         <v>32</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F9" s="27"/>
       <c r="G9" s="44"/>
@@ -1751,10 +1790,10 @@
         <v>33</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F10" s="27"/>
       <c r="G10" s="37"/>
@@ -1784,7 +1823,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="44"/>
@@ -1838,13 +1877,13 @@
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="49" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F13" s="49"/>
       <c r="G13" s="44"/>
@@ -2043,7 +2082,7 @@
       <c r="T19" s="34"/>
     </row>
     <row r="20" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24">
+      <c r="A20" s="46">
         <v>16</v>
       </c>
       <c r="B20" s="25"/>
@@ -2111,18 +2150,18 @@
       <c r="N22" s="56"/>
     </row>
     <row r="23" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
+      <c r="B23" s="80"/>
+      <c r="C23" s="80"/>
       <c r="D23" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="79" t="s">
+      <c r="E23" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="79"/>
+      <c r="F23" s="81"/>
       <c r="G23" s="13"/>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
@@ -2139,18 +2178,18 @@
       <c r="T23" s="18"/>
     </row>
     <row r="24" spans="1:20" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
       <c r="D24" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="80" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="80"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
       <c r="I24" s="22"/>
@@ -2174,7 +2213,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>20</v>
@@ -2208,14 +2247,14 @@
         <v>25</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="28"/>
       <c r="F26" s="37" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
@@ -2233,12 +2272,10 @@
       <c r="T26" s="34"/>
     </row>
     <row r="27" spans="1:20" s="35" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
-        <v>5</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>25</v>
-      </c>
+      <c r="A27" s="46">
+        <v>3</v>
+      </c>
+      <c r="B27" s="25"/>
       <c r="C27" s="48" t="s">
         <v>70</v>
       </c>
@@ -2246,11 +2283,9 @@
         <v>20</v>
       </c>
       <c r="E27" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="51" t="s">
-        <v>80</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="F27" s="51"/>
       <c r="G27" s="38"/>
       <c r="H27" s="39"/>
       <c r="I27" s="42"/>
@@ -2267,8 +2302,8 @@
       <c r="T27" s="34"/>
     </row>
     <row r="28" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="24">
-        <v>6</v>
+      <c r="A28" s="46">
+        <v>4</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="43" t="s">
@@ -2297,8 +2332,8 @@
       <c r="T28" s="18"/>
     </row>
     <row r="29" spans="1:20" s="35" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
-        <v>7</v>
+      <c r="A29" s="46">
+        <v>5</v>
       </c>
       <c r="B29" s="25"/>
       <c r="C29" s="48" t="s">
@@ -2327,18 +2362,18 @@
       <c r="T29" s="34"/>
     </row>
     <row r="30" spans="1:20" s="35" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="24">
-        <v>9</v>
+      <c r="A30" s="46">
+        <v>6</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="43" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E30" s="59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F30" s="49"/>
       <c r="G30" s="44"/>
@@ -2357,18 +2392,18 @@
       <c r="T30" s="34"/>
     </row>
     <row r="31" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24">
-        <v>10</v>
+      <c r="A31" s="46">
+        <v>7</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="43" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F31" s="49"/>
       <c r="G31" s="37"/>
@@ -2387,8 +2422,8 @@
       <c r="T31" s="18"/>
     </row>
     <row r="32" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="24">
-        <v>12</v>
+      <c r="A32" s="46">
+        <v>8</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="48" t="s">
@@ -2398,7 +2433,7 @@
         <v>23</v>
       </c>
       <c r="E32" s="50" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F32" s="49"/>
       <c r="G32" s="44"/>
@@ -2417,8 +2452,8 @@
       <c r="T32" s="18"/>
     </row>
     <row r="33" spans="1:20" s="35" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24">
-        <v>13</v>
+      <c r="A33" s="46">
+        <v>9</v>
       </c>
       <c r="B33" s="47"/>
       <c r="C33" s="48" t="s">
@@ -2447,16 +2482,18 @@
       <c r="T33" s="34"/>
     </row>
     <row r="34" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="46"/>
+      <c r="A34" s="46">
+        <v>10</v>
+      </c>
       <c r="B34" s="47"/>
       <c r="C34" s="48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D34" s="49" t="s">
         <v>20</v>
       </c>
       <c r="E34" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F34" s="49"/>
       <c r="G34" s="44"/>
@@ -2475,8 +2512,8 @@
       <c r="T34" s="18"/>
     </row>
     <row r="35" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24">
-        <v>14</v>
+      <c r="A35" s="46">
+        <v>11</v>
       </c>
       <c r="B35" s="25"/>
       <c r="C35" s="43" t="s">
@@ -2505,8 +2542,8 @@
       <c r="T35" s="18"/>
     </row>
     <row r="36" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24">
-        <v>15</v>
+      <c r="A36" s="46">
+        <v>12</v>
       </c>
       <c r="B36" s="25"/>
       <c r="C36" s="43" t="s">
@@ -2535,8 +2572,8 @@
       <c r="T36" s="18"/>
     </row>
     <row r="37" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="24">
-        <v>16</v>
+      <c r="A37" s="46">
+        <v>13</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="43" t="s">
@@ -2565,8 +2602,8 @@
       <c r="T37" s="18"/>
     </row>
     <row r="38" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="24">
-        <v>17</v>
+      <c r="A38" s="46">
+        <v>14</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="43" t="s">
@@ -2595,8 +2632,8 @@
       <c r="T38" s="18"/>
     </row>
     <row r="39" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24">
-        <v>18</v>
+      <c r="A39" s="46">
+        <v>15</v>
       </c>
       <c r="B39" s="25"/>
       <c r="C39" s="43" t="s">
@@ -2625,8 +2662,8 @@
       <c r="T39" s="18"/>
     </row>
     <row r="40" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="24">
-        <v>19</v>
+      <c r="A40" s="46">
+        <v>16</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="43" t="s">
@@ -2655,8 +2692,8 @@
       <c r="T40" s="18"/>
     </row>
     <row r="41" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="24">
-        <v>20</v>
+      <c r="A41" s="46">
+        <v>17</v>
       </c>
       <c r="B41" s="25"/>
       <c r="C41" s="43" t="s">
@@ -2723,18 +2760,18 @@
       <c r="N43" s="56"/>
     </row>
     <row r="44" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A44" s="77" t="s">
+      <c r="A44" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B44" s="77"/>
-      <c r="C44" s="77"/>
+      <c r="B44" s="80"/>
+      <c r="C44" s="80"/>
       <c r="D44" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E44" s="79" t="s">
+      <c r="E44" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="F44" s="79"/>
+      <c r="F44" s="81"/>
       <c r="G44" s="13"/>
       <c r="H44" s="14"/>
       <c r="I44" s="15"/>
@@ -2751,18 +2788,18 @@
       <c r="T44" s="18"/>
     </row>
     <row r="45" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="73" t="s">
+      <c r="A45" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73"/>
+      <c r="B45" s="83"/>
+      <c r="C45" s="83"/>
       <c r="D45" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="74" t="s">
+      <c r="E45" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="F45" s="74"/>
+      <c r="F45" s="84"/>
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
       <c r="I45" s="60"/>
@@ -3006,7 +3043,7 @@
       <c r="S53" s="18"/>
       <c r="T53" s="18"/>
     </row>
-    <row r="54" spans="1:20" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="66"/>
       <c r="B54" s="67"/>
       <c r="C54" s="67"/>
@@ -3022,27 +3059,27 @@
       <c r="M54" s="53"/>
       <c r="N54" s="56"/>
     </row>
-    <row r="55" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B55" s="77"/>
-      <c r="C55" s="77"/>
-      <c r="D55" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="F55" s="78"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="16"/>
+    <row r="55" spans="1:20" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" s="83"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="84" t="s">
+        <v>94</v>
+      </c>
+      <c r="F55" s="84"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="73"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="60"/>
+      <c r="K55" s="60"/>
+      <c r="L55" s="60"/>
+      <c r="M55" s="60"/>
+      <c r="N55" s="61"/>
       <c r="O55" s="17"/>
       <c r="P55" s="18"/>
       <c r="Q55" s="18"/>
@@ -3050,27 +3087,33 @@
       <c r="S55" s="18"/>
       <c r="T55" s="18"/>
     </row>
-    <row r="56" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A56" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" s="73"/>
-      <c r="C56" s="73"/>
-      <c r="D56" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E56" s="74" t="s">
-        <v>59</v>
-      </c>
-      <c r="F56" s="74"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="23"/>
+    <row r="56" spans="1:20" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="46">
+        <v>1</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="38"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="62"/>
+      <c r="J56" s="62"/>
+      <c r="K56" s="62"/>
+      <c r="L56" s="62"/>
+      <c r="M56" s="62"/>
+      <c r="N56" s="63"/>
       <c r="O56" s="17"/>
       <c r="P56" s="18"/>
       <c r="Q56" s="18"/>
@@ -3078,24 +3121,22 @@
       <c r="S56" s="18"/>
       <c r="T56" s="18"/>
     </row>
-    <row r="57" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="24">
-        <v>1</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57" s="27" t="s">
+    <row r="57" spans="1:20" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="46">
+        <v>2</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" s="27" t="s">
-        <v>22</v>
+      <c r="E57" s="50"/>
+      <c r="F57" s="51" t="s">
+        <v>96</v>
       </c>
       <c r="G57" s="38"/>
       <c r="H57" s="30"/>
@@ -3112,23 +3153,21 @@
       <c r="S57" s="18"/>
       <c r="T57" s="18"/>
     </row>
-    <row r="58" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="24">
-        <v>2</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58" s="28"/>
-      <c r="F58" s="37" t="s">
-        <v>84</v>
-      </c>
+    <row r="58" spans="1:20" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="46">
+        <v>3</v>
+      </c>
+      <c r="B58" s="47"/>
+      <c r="C58" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" s="51"/>
       <c r="G58" s="38"/>
       <c r="H58" s="30"/>
       <c r="I58" s="62"/>
@@ -3145,20 +3184,20 @@
       <c r="T58" s="18"/>
     </row>
     <row r="59" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="24">
-        <v>3</v>
-      </c>
-      <c r="B59" s="25"/>
+      <c r="A59" s="46">
+        <v>4</v>
+      </c>
+      <c r="B59" s="47"/>
       <c r="C59" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E59" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="F59" s="27"/>
+        <v>54</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="49"/>
       <c r="G59" s="38"/>
       <c r="H59" s="39"/>
       <c r="I59" s="65"/>
@@ -3175,20 +3214,20 @@
       <c r="T59" s="18"/>
     </row>
     <row r="60" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="24">
-        <v>4</v>
-      </c>
-      <c r="B60" s="25"/>
+      <c r="A60" s="46">
+        <v>5</v>
+      </c>
+      <c r="B60" s="47"/>
       <c r="C60" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E60" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="F60" s="27"/>
+        <v>56</v>
+      </c>
+      <c r="D60" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F60" s="49"/>
       <c r="G60" s="38"/>
       <c r="H60" s="39"/>
       <c r="I60" s="62"/>
@@ -3204,21 +3243,21 @@
       <c r="S60" s="18"/>
       <c r="T60" s="18"/>
     </row>
-    <row r="61" spans="1:20" s="1" customFormat="1" ht="21" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="24">
-        <v>5</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E61" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="F61" s="27"/>
+    <row r="61" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="46">
+        <v>6</v>
+      </c>
+      <c r="B61" s="47"/>
+      <c r="C61" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="D61" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E61" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F61" s="49"/>
       <c r="G61" s="44"/>
       <c r="H61" s="39"/>
       <c r="I61" s="65"/>
@@ -3235,20 +3274,20 @@
       <c r="T61" s="18"/>
     </row>
     <row r="62" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="24">
-        <v>6</v>
-      </c>
-      <c r="B62" s="25"/>
+      <c r="A62" s="46">
+        <v>7</v>
+      </c>
+      <c r="B62" s="47"/>
       <c r="C62" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E62" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="F62" s="27"/>
+        <v>58</v>
+      </c>
+      <c r="D62" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" s="49"/>
       <c r="G62" s="44"/>
       <c r="H62" s="39"/>
       <c r="I62" s="62"/>
@@ -3264,28 +3303,20 @@
       <c r="S62" s="18"/>
       <c r="T62" s="18"/>
     </row>
-    <row r="63" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="24">
-        <v>7</v>
-      </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E63" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="F63" s="27"/>
+    <row r="63" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="46"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="49"/>
       <c r="G63" s="44"/>
       <c r="H63" s="39"/>
-      <c r="I63" s="62"/>
-      <c r="J63" s="62"/>
-      <c r="K63" s="62"/>
-      <c r="L63" s="62"/>
-      <c r="M63" s="62"/>
+      <c r="I63" s="65"/>
+      <c r="J63" s="65"/>
+      <c r="K63" s="65"/>
+      <c r="L63" s="65"/>
+      <c r="M63" s="65"/>
       <c r="N63" s="64"/>
       <c r="O63" s="17"/>
       <c r="P63" s="18"/>
@@ -3294,21 +3325,13 @@
       <c r="S63" s="18"/>
       <c r="T63" s="18"/>
     </row>
-    <row r="64" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24">
-        <v>8</v>
-      </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E64" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="F64" s="27"/>
+    <row r="64" spans="1:20" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="46"/>
+      <c r="B64" s="47"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="49"/>
       <c r="G64" s="44"/>
       <c r="H64" s="39"/>
       <c r="I64" s="62"/>
@@ -3324,51 +3347,43 @@
       <c r="S64" s="18"/>
       <c r="T64" s="18"/>
     </row>
-    <row r="65" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="24">
-        <v>9</v>
-      </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="E65" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="F65" s="27"/>
-      <c r="G65" s="44"/>
-      <c r="H65" s="39"/>
-      <c r="I65" s="65"/>
-      <c r="J65" s="65"/>
-      <c r="K65" s="65"/>
-      <c r="L65" s="65"/>
-      <c r="M65" s="65"/>
-      <c r="N65" s="64"/>
-      <c r="O65" s="17"/>
-      <c r="P65" s="18"/>
-      <c r="Q65" s="18"/>
-      <c r="R65" s="18"/>
-      <c r="S65" s="18"/>
-      <c r="T65" s="18"/>
-    </row>
-    <row r="66" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="24"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="43"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="62"/>
-      <c r="L66" s="62"/>
-      <c r="M66" s="62"/>
-      <c r="N66" s="64"/>
+    <row r="65" spans="1:20" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="66"/>
+      <c r="B65" s="67"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="67"/>
+      <c r="G65" s="55"/>
+      <c r="H65" s="69"/>
+      <c r="I65" s="53"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="53"/>
+      <c r="L65" s="53"/>
+      <c r="M65" s="53"/>
+      <c r="N65" s="56"/>
+    </row>
+    <row r="66" spans="1:20" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" s="80"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" s="85"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="16"/>
       <c r="O66" s="17"/>
       <c r="P66" s="18"/>
       <c r="Q66" s="18"/>
@@ -3376,43 +3391,61 @@
       <c r="S66" s="18"/>
       <c r="T66" s="18"/>
     </row>
-    <row r="67" spans="1:20" s="1" customFormat="1" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="66"/>
-      <c r="B67" s="67"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="67"/>
-      <c r="G67" s="55"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="53"/>
-      <c r="J67" s="53"/>
-      <c r="K67" s="53"/>
-      <c r="L67" s="53"/>
-      <c r="M67" s="53"/>
-      <c r="N67" s="56"/>
-    </row>
-    <row r="68" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B68" s="77"/>
-      <c r="C68" s="77"/>
-      <c r="D68" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E68" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="F68" s="78"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="15"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="16"/>
+    <row r="67" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="83"/>
+      <c r="C67" s="83"/>
+      <c r="D67" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E67" s="84" t="s">
+        <v>59</v>
+      </c>
+      <c r="F67" s="84"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+      <c r="L67" s="22"/>
+      <c r="M67" s="22"/>
+      <c r="N67" s="23"/>
+      <c r="O67" s="17"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
+      <c r="S67" s="18"/>
+      <c r="T67" s="18"/>
+    </row>
+    <row r="68" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="24">
+        <v>1</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F68" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="38"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="62"/>
+      <c r="J68" s="62"/>
+      <c r="K68" s="62"/>
+      <c r="L68" s="62"/>
+      <c r="M68" s="62"/>
+      <c r="N68" s="63"/>
       <c r="O68" s="17"/>
       <c r="P68" s="18"/>
       <c r="Q68" s="18"/>
@@ -3420,27 +3453,31 @@
       <c r="S68" s="18"/>
       <c r="T68" s="18"/>
     </row>
-    <row r="69" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="B69" s="73"/>
-      <c r="C69" s="73"/>
-      <c r="D69" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="E69" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="F69" s="76"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="22"/>
-      <c r="K69" s="22"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="22"/>
-      <c r="N69" s="23"/>
+    <row r="69" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="24">
+        <v>2</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E69" s="28"/>
+      <c r="F69" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="G69" s="38"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="62"/>
+      <c r="J69" s="62"/>
+      <c r="K69" s="62"/>
+      <c r="L69" s="62"/>
+      <c r="M69" s="62"/>
+      <c r="N69" s="64"/>
       <c r="O69" s="17"/>
       <c r="P69" s="18"/>
       <c r="Q69" s="18"/>
@@ -3448,151 +3485,149 @@
       <c r="S69" s="18"/>
       <c r="T69" s="18"/>
     </row>
-    <row r="70" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A70" s="24">
-        <v>1</v>
-      </c>
-      <c r="B70" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" s="26" t="s">
-        <v>91</v>
+        <v>3</v>
+      </c>
+      <c r="B70" s="25"/>
+      <c r="C70" s="43" t="s">
+        <v>60</v>
       </c>
       <c r="D70" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E70" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="F70" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="G70" s="29"/>
-      <c r="H70" s="30"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
-      <c r="K70" s="31"/>
-      <c r="L70" s="31"/>
-      <c r="M70" s="31"/>
-      <c r="N70" s="32"/>
-      <c r="O70" s="33"/>
-      <c r="P70" s="34"/>
-      <c r="Q70" s="34"/>
-      <c r="R70" s="34"/>
-      <c r="S70" s="34"/>
-      <c r="T70" s="34"/>
-    </row>
-    <row r="71" spans="1:20" s="35" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="46">
-        <v>2</v>
-      </c>
-      <c r="B71" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="D71" s="49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71" s="50" t="s">
-        <v>92</v>
-      </c>
-      <c r="F71" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="G71" s="29"/>
-      <c r="H71" s="30"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
-      <c r="L71" s="31"/>
-      <c r="M71" s="31"/>
-      <c r="N71" s="32"/>
-      <c r="O71" s="33"/>
-      <c r="P71" s="34"/>
-      <c r="Q71" s="34"/>
-      <c r="R71" s="34"/>
-      <c r="S71" s="34"/>
-      <c r="T71" s="34"/>
-    </row>
-    <row r="72" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="24"/>
+      <c r="E70" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" s="27"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="39"/>
+      <c r="I70" s="65"/>
+      <c r="J70" s="65"/>
+      <c r="K70" s="65"/>
+      <c r="L70" s="65"/>
+      <c r="M70" s="65"/>
+      <c r="N70" s="64"/>
+      <c r="O70" s="17"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="18"/>
+      <c r="R70" s="18"/>
+      <c r="S70" s="18"/>
+      <c r="T70" s="18"/>
+    </row>
+    <row r="71" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="24">
+        <v>4</v>
+      </c>
+      <c r="B71" s="25"/>
+      <c r="C71" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E71" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F71" s="27"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="62"/>
+      <c r="K71" s="62"/>
+      <c r="L71" s="62"/>
+      <c r="M71" s="62"/>
+      <c r="N71" s="64"/>
+      <c r="O71" s="17"/>
+      <c r="P71" s="18"/>
+      <c r="Q71" s="18"/>
+      <c r="R71" s="18"/>
+      <c r="S71" s="18"/>
+      <c r="T71" s="18"/>
+    </row>
+    <row r="72" spans="1:20" s="1" customFormat="1" ht="21" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="24">
+        <v>5</v>
+      </c>
       <c r="B72" s="25"/>
-      <c r="C72" s="83" t="s">
-        <v>93</v>
-      </c>
-      <c r="D72" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="E72" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="F72" s="37"/>
-      <c r="G72" s="38"/>
+      <c r="C72" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F72" s="27"/>
+      <c r="G72" s="44"/>
       <c r="H72" s="39"/>
-      <c r="I72" s="31"/>
-      <c r="J72" s="31"/>
-      <c r="K72" s="31"/>
-      <c r="L72" s="31"/>
-      <c r="M72" s="31"/>
-      <c r="N72" s="40"/>
-      <c r="O72" s="33"/>
-      <c r="P72" s="34"/>
-      <c r="Q72" s="34"/>
-      <c r="R72" s="34"/>
-      <c r="S72" s="34"/>
-      <c r="T72" s="34"/>
-    </row>
-    <row r="73" spans="1:20" s="35" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="24"/>
+      <c r="I72" s="65"/>
+      <c r="J72" s="65"/>
+      <c r="K72" s="65"/>
+      <c r="L72" s="65"/>
+      <c r="M72" s="65"/>
+      <c r="N72" s="64"/>
+      <c r="O72" s="17"/>
+      <c r="P72" s="18"/>
+      <c r="Q72" s="18"/>
+      <c r="R72" s="18"/>
+      <c r="S72" s="18"/>
+      <c r="T72" s="18"/>
+    </row>
+    <row r="73" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="24">
+        <v>6</v>
+      </c>
       <c r="B73" s="25"/>
-      <c r="C73" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="E73" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="F73" s="37"/>
-      <c r="G73" s="38"/>
+      <c r="C73" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E73" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" s="27"/>
+      <c r="G73" s="44"/>
       <c r="H73" s="39"/>
-      <c r="I73" s="42"/>
-      <c r="J73" s="42"/>
-      <c r="K73" s="42"/>
-      <c r="L73" s="42"/>
-      <c r="M73" s="42"/>
-      <c r="N73" s="40"/>
-      <c r="O73" s="33"/>
-      <c r="P73" s="34"/>
-      <c r="Q73" s="34"/>
-      <c r="R73" s="34"/>
-      <c r="S73" s="34"/>
-      <c r="T73" s="34"/>
-    </row>
-    <row r="74" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="24"/>
+      <c r="I73" s="62"/>
+      <c r="J73" s="62"/>
+      <c r="K73" s="62"/>
+      <c r="L73" s="62"/>
+      <c r="M73" s="62"/>
+      <c r="N73" s="64"/>
+      <c r="O73" s="17"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" s="18"/>
+    </row>
+    <row r="74" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="24">
+        <v>7</v>
+      </c>
       <c r="B74" s="25"/>
       <c r="C74" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="D74" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="E74" s="43" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" s="41" t="s">
+        <v>47</v>
       </c>
       <c r="F74" s="27"/>
-      <c r="G74" s="37"/>
+      <c r="G74" s="44"/>
       <c r="H74" s="39"/>
-      <c r="I74" s="31"/>
-      <c r="J74" s="31"/>
-      <c r="K74" s="31"/>
-      <c r="L74" s="31"/>
-      <c r="M74" s="31"/>
-      <c r="N74" s="40"/>
+      <c r="I74" s="62"/>
+      <c r="J74" s="62"/>
+      <c r="K74" s="62"/>
+      <c r="L74" s="62"/>
+      <c r="M74" s="62"/>
+      <c r="N74" s="64"/>
       <c r="O74" s="17"/>
       <c r="P74" s="18"/>
       <c r="Q74" s="18"/>
@@ -3600,55 +3635,59 @@
       <c r="S74" s="18"/>
       <c r="T74" s="18"/>
     </row>
-    <row r="75" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="24"/>
+    <row r="75" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24">
+        <v>8</v>
+      </c>
       <c r="B75" s="25"/>
       <c r="C75" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E75" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="F75" s="37"/>
-      <c r="G75" s="37"/>
+        <v>48</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F75" s="27"/>
+      <c r="G75" s="44"/>
       <c r="H75" s="39"/>
-      <c r="I75" s="42"/>
-      <c r="J75" s="42"/>
-      <c r="K75" s="42"/>
-      <c r="L75" s="42"/>
-      <c r="M75" s="42"/>
-      <c r="N75" s="40"/>
-      <c r="O75" s="33"/>
-      <c r="P75" s="34"/>
-      <c r="Q75" s="34"/>
-      <c r="R75" s="34"/>
-      <c r="S75" s="34"/>
-      <c r="T75" s="34"/>
-    </row>
-    <row r="76" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="62"/>
+      <c r="K75" s="62"/>
+      <c r="L75" s="62"/>
+      <c r="M75" s="62"/>
+      <c r="N75" s="64"/>
+      <c r="O75" s="17"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="18"/>
+      <c r="R75" s="18"/>
+      <c r="S75" s="18"/>
+      <c r="T75" s="18"/>
+    </row>
+    <row r="76" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24">
+        <v>9</v>
+      </c>
       <c r="B76" s="25"/>
       <c r="C76" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D76" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="E76" s="59" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="D76" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="41" t="s">
+        <v>51</v>
       </c>
       <c r="F76" s="27"/>
       <c r="G76" s="44"/>
       <c r="H76" s="39"/>
-      <c r="I76" s="31"/>
-      <c r="J76" s="31"/>
-      <c r="K76" s="31"/>
-      <c r="L76" s="31"/>
-      <c r="M76" s="31"/>
-      <c r="N76" s="40"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="65"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="65"/>
+      <c r="M76" s="65"/>
+      <c r="N76" s="64"/>
       <c r="O76" s="17"/>
       <c r="P76" s="18"/>
       <c r="Q76" s="18"/>
@@ -3656,93 +3695,99 @@
       <c r="S76" s="18"/>
       <c r="T76" s="18"/>
     </row>
-    <row r="77" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A77" s="24"/>
       <c r="B77" s="25"/>
-      <c r="C77" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E77" s="59" t="s">
-        <v>51</v>
-      </c>
+      <c r="C77" s="43"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="28"/>
       <c r="F77" s="27"/>
       <c r="G77" s="44"/>
       <c r="H77" s="39"/>
-      <c r="I77" s="42"/>
-      <c r="J77" s="42"/>
-      <c r="K77" s="42"/>
-      <c r="L77" s="42"/>
-      <c r="M77" s="42"/>
-      <c r="N77" s="40"/>
-      <c r="O77" s="33"/>
-      <c r="P77" s="34"/>
-      <c r="Q77" s="34"/>
-      <c r="R77" s="34"/>
-      <c r="S77" s="34"/>
-      <c r="T77" s="34"/>
-    </row>
-    <row r="78" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="43"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="39"/>
-      <c r="I78" s="31"/>
-      <c r="J78" s="31"/>
-      <c r="K78" s="31"/>
-      <c r="L78" s="31"/>
-      <c r="M78" s="31"/>
-      <c r="N78" s="40"/>
-      <c r="O78" s="17"/>
-      <c r="P78" s="18"/>
-      <c r="Q78" s="18"/>
-      <c r="R78" s="18"/>
-      <c r="S78" s="18"/>
-      <c r="T78" s="18"/>
-    </row>
-    <row r="79" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="24"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="27"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="37"/>
-      <c r="G79" s="37"/>
-      <c r="H79" s="39"/>
-      <c r="I79" s="42"/>
-      <c r="J79" s="42"/>
-      <c r="K79" s="42"/>
-      <c r="L79" s="42"/>
-      <c r="M79" s="42"/>
-      <c r="N79" s="40"/>
-      <c r="O79" s="33"/>
-      <c r="P79" s="34"/>
-      <c r="Q79" s="34"/>
-      <c r="R79" s="34"/>
-      <c r="S79" s="34"/>
-      <c r="T79" s="34"/>
-    </row>
-    <row r="80" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="24"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="27"/>
-      <c r="E80" s="28"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="39"/>
-      <c r="I80" s="31"/>
-      <c r="J80" s="31"/>
-      <c r="K80" s="31"/>
-      <c r="L80" s="31"/>
-      <c r="M80" s="31"/>
-      <c r="N80" s="40"/>
+      <c r="I77" s="62"/>
+      <c r="J77" s="62"/>
+      <c r="K77" s="62"/>
+      <c r="L77" s="62"/>
+      <c r="M77" s="62"/>
+      <c r="N77" s="64"/>
+      <c r="O77" s="17"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="18"/>
+      <c r="R77" s="18"/>
+      <c r="S77" s="18"/>
+      <c r="T77" s="18"/>
+    </row>
+    <row r="78" spans="1:20" s="1" customFormat="1" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="66"/>
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="68"/>
+      <c r="F78" s="67"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="69"/>
+      <c r="I78" s="53"/>
+      <c r="J78" s="53"/>
+      <c r="K78" s="53"/>
+      <c r="L78" s="53"/>
+      <c r="M78" s="53"/>
+      <c r="N78" s="56"/>
+    </row>
+    <row r="79" spans="1:20" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B79" s="83"/>
+      <c r="C79" s="83"/>
+      <c r="D79" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="E79" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="F79" s="84"/>
+      <c r="G79" s="73"/>
+      <c r="H79" s="73"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="22"/>
+      <c r="L79" s="22"/>
+      <c r="M79" s="22"/>
+      <c r="N79" s="23"/>
+      <c r="O79" s="17"/>
+      <c r="P79" s="18"/>
+      <c r="Q79" s="18"/>
+      <c r="R79" s="18"/>
+      <c r="S79" s="18"/>
+      <c r="T79" s="18"/>
+    </row>
+    <row r="80" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="46">
+        <v>1</v>
+      </c>
+      <c r="B80" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="D80" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F80" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" s="38"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="62"/>
+      <c r="J80" s="62"/>
+      <c r="K80" s="62"/>
+      <c r="L80" s="62"/>
+      <c r="M80" s="62"/>
+      <c r="N80" s="63"/>
       <c r="O80" s="17"/>
       <c r="P80" s="18"/>
       <c r="Q80" s="18"/>
@@ -3750,21 +3795,31 @@
       <c r="S80" s="18"/>
       <c r="T80" s="18"/>
     </row>
-    <row r="81" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="46"/>
-      <c r="B81" s="47"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="49"/>
-      <c r="E81" s="59"/>
-      <c r="F81" s="51"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="39"/>
-      <c r="I81" s="31"/>
-      <c r="J81" s="31"/>
-      <c r="K81" s="31"/>
-      <c r="L81" s="31"/>
-      <c r="M81" s="31"/>
-      <c r="N81" s="40"/>
+    <row r="81" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="46">
+        <v>2</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D81" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E81" s="50"/>
+      <c r="F81" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G81" s="38"/>
+      <c r="H81" s="30"/>
+      <c r="I81" s="62"/>
+      <c r="J81" s="62"/>
+      <c r="K81" s="62"/>
+      <c r="L81" s="62"/>
+      <c r="M81" s="62"/>
+      <c r="N81" s="63"/>
       <c r="O81" s="17"/>
       <c r="P81" s="18"/>
       <c r="Q81" s="18"/>
@@ -3772,43 +3827,57 @@
       <c r="S81" s="18"/>
       <c r="T81" s="18"/>
     </row>
-    <row r="82" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="24"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="41"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="39"/>
-      <c r="I82" s="42"/>
-      <c r="J82" s="42"/>
-      <c r="K82" s="42"/>
-      <c r="L82" s="42"/>
-      <c r="M82" s="42"/>
-      <c r="N82" s="40"/>
-      <c r="O82" s="33"/>
-      <c r="P82" s="34"/>
-      <c r="Q82" s="34"/>
-      <c r="R82" s="34"/>
-      <c r="S82" s="34"/>
-      <c r="T82" s="34"/>
-    </row>
-    <row r="83" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="46"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="41"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="37"/>
+    <row r="82" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="46">
+        <v>3</v>
+      </c>
+      <c r="B82" s="47"/>
+      <c r="C82" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D82" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E82" s="50"/>
+      <c r="F82" s="51"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="30"/>
+      <c r="I82" s="62"/>
+      <c r="J82" s="62"/>
+      <c r="K82" s="62"/>
+      <c r="L82" s="62"/>
+      <c r="M82" s="62"/>
+      <c r="N82" s="64"/>
+      <c r="O82" s="17"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="18"/>
+      <c r="R82" s="18"/>
+      <c r="S82" s="18"/>
+      <c r="T82" s="18"/>
+    </row>
+    <row r="83" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="46">
+        <v>4</v>
+      </c>
+      <c r="B83" s="47"/>
+      <c r="C83" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E83" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F83" s="49"/>
+      <c r="G83" s="38"/>
       <c r="H83" s="39"/>
-      <c r="I83" s="31"/>
-      <c r="J83" s="31"/>
-      <c r="K83" s="31"/>
-      <c r="L83" s="31"/>
-      <c r="M83" s="31"/>
-      <c r="N83" s="40"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
+      <c r="L83" s="65"/>
+      <c r="M83" s="65"/>
+      <c r="N83" s="64"/>
       <c r="O83" s="17"/>
       <c r="P83" s="18"/>
       <c r="Q83" s="18"/>
@@ -3816,65 +3885,89 @@
       <c r="S83" s="18"/>
       <c r="T83" s="18"/>
     </row>
-    <row r="84" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="24"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="43"/>
-      <c r="D84" s="27"/>
-      <c r="E84" s="28"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="44"/>
+    <row r="84" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="46">
+        <v>5</v>
+      </c>
+      <c r="B84" s="47"/>
+      <c r="C84" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D84" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E84" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="F84" s="49"/>
+      <c r="G84" s="38"/>
       <c r="H84" s="39"/>
-      <c r="I84" s="42"/>
-      <c r="J84" s="42"/>
-      <c r="K84" s="42"/>
-      <c r="L84" s="42"/>
-      <c r="M84" s="42"/>
-      <c r="N84" s="40"/>
-      <c r="O84" s="33"/>
-      <c r="P84" s="34"/>
-      <c r="Q84" s="34"/>
-      <c r="R84" s="34"/>
-      <c r="S84" s="34"/>
-      <c r="T84" s="34"/>
-    </row>
-    <row r="85" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="46"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="43"/>
-      <c r="D85" s="27"/>
-      <c r="E85" s="41"/>
-      <c r="F85" s="27"/>
+      <c r="I84" s="62"/>
+      <c r="J84" s="62"/>
+      <c r="K84" s="62"/>
+      <c r="L84" s="62"/>
+      <c r="M84" s="62"/>
+      <c r="N84" s="64"/>
+      <c r="O84" s="17"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="18"/>
+      <c r="R84" s="18"/>
+      <c r="S84" s="18"/>
+      <c r="T84" s="18"/>
+    </row>
+    <row r="85" spans="1:20" s="1" customFormat="1" ht="21" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="46">
+        <v>6</v>
+      </c>
+      <c r="B85" s="47"/>
+      <c r="C85" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F85" s="49"/>
       <c r="G85" s="44"/>
       <c r="H85" s="39"/>
-      <c r="I85" s="42"/>
-      <c r="J85" s="42"/>
-      <c r="K85" s="42"/>
-      <c r="L85" s="42"/>
-      <c r="M85" s="42"/>
-      <c r="N85" s="40"/>
-      <c r="O85" s="33"/>
-      <c r="P85" s="34"/>
-      <c r="Q85" s="34"/>
-      <c r="R85" s="34"/>
-      <c r="S85" s="34"/>
-      <c r="T85" s="34"/>
-    </row>
-    <row r="86" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="24"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="43"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="41"/>
-      <c r="F86" s="27"/>
-      <c r="G86" s="37"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="65"/>
+      <c r="L85" s="65"/>
+      <c r="M85" s="65"/>
+      <c r="N85" s="64"/>
+      <c r="O85" s="17"/>
+      <c r="P85" s="18"/>
+      <c r="Q85" s="18"/>
+      <c r="R85" s="18"/>
+      <c r="S85" s="18"/>
+      <c r="T85" s="18"/>
+    </row>
+    <row r="86" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="46">
+        <v>7</v>
+      </c>
+      <c r="B86" s="47"/>
+      <c r="C86" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E86" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" s="49"/>
+      <c r="G86" s="44"/>
       <c r="H86" s="39"/>
-      <c r="I86" s="31"/>
-      <c r="J86" s="31"/>
-      <c r="K86" s="31"/>
-      <c r="L86" s="31"/>
-      <c r="M86" s="31"/>
-      <c r="N86" s="40"/>
+      <c r="I86" s="62"/>
+      <c r="J86" s="62"/>
+      <c r="K86" s="62"/>
+      <c r="L86" s="62"/>
+      <c r="M86" s="62"/>
+      <c r="N86" s="64"/>
       <c r="O86" s="17"/>
       <c r="P86" s="18"/>
       <c r="Q86" s="18"/>
@@ -3882,21 +3975,29 @@
       <c r="S86" s="18"/>
       <c r="T86" s="18"/>
     </row>
-    <row r="87" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="24"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="30"/>
+    <row r="87" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="46">
+        <v>8</v>
+      </c>
+      <c r="B87" s="47"/>
+      <c r="C87" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D87" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F87" s="49"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="39"/>
       <c r="I87" s="62"/>
       <c r="J87" s="62"/>
       <c r="K87" s="62"/>
       <c r="L87" s="62"/>
       <c r="M87" s="62"/>
-      <c r="N87" s="63"/>
+      <c r="N87" s="64"/>
       <c r="O87" s="17"/>
       <c r="P87" s="18"/>
       <c r="Q87" s="18"/>
@@ -3904,37 +4005,59 @@
       <c r="S87" s="18"/>
       <c r="T87" s="18"/>
     </row>
-    <row r="88" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="66"/>
-      <c r="B88" s="67"/>
-      <c r="C88" s="67"/>
-      <c r="D88" s="67"/>
-      <c r="E88" s="68"/>
-      <c r="F88" s="67"/>
-      <c r="G88" s="67"/>
-      <c r="H88" s="67"/>
-      <c r="I88" s="67"/>
-      <c r="J88" s="67"/>
-      <c r="K88" s="67"/>
-      <c r="L88" s="67"/>
-      <c r="M88" s="67"/>
-      <c r="N88" s="71"/>
-    </row>
-    <row r="89" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A89" s="77"/>
-      <c r="B89" s="77"/>
-      <c r="C89" s="77"/>
-      <c r="D89" s="57"/>
-      <c r="E89" s="79"/>
-      <c r="F89" s="79"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="14"/>
-      <c r="I89" s="15"/>
-      <c r="J89" s="15"/>
-      <c r="K89" s="15"/>
-      <c r="L89" s="15"/>
-      <c r="M89" s="15"/>
-      <c r="N89" s="16"/>
+    <row r="88" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="46">
+        <v>9</v>
+      </c>
+      <c r="B88" s="47"/>
+      <c r="C88" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D88" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E88" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F88" s="49"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="39"/>
+      <c r="I88" s="62"/>
+      <c r="J88" s="62"/>
+      <c r="K88" s="62"/>
+      <c r="L88" s="62"/>
+      <c r="M88" s="62"/>
+      <c r="N88" s="64"/>
+      <c r="O88" s="17"/>
+      <c r="P88" s="18"/>
+      <c r="Q88" s="18"/>
+      <c r="R88" s="18"/>
+      <c r="S88" s="18"/>
+      <c r="T88" s="18"/>
+    </row>
+    <row r="89" spans="1:20" s="1" customFormat="1" ht="18" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="46">
+        <v>10</v>
+      </c>
+      <c r="B89" s="47"/>
+      <c r="C89" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D89" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E89" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F89" s="49"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="39"/>
+      <c r="I89" s="65"/>
+      <c r="J89" s="65"/>
+      <c r="K89" s="65"/>
+      <c r="L89" s="65"/>
+      <c r="M89" s="65"/>
+      <c r="N89" s="64"/>
       <c r="O89" s="17"/>
       <c r="P89" s="18"/>
       <c r="Q89" s="18"/>
@@ -3942,21 +4065,21 @@
       <c r="S89" s="18"/>
       <c r="T89" s="18"/>
     </row>
-    <row r="90" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A90" s="73"/>
-      <c r="B90" s="73"/>
-      <c r="C90" s="73"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="74"/>
-      <c r="F90" s="74"/>
-      <c r="G90" s="21"/>
-      <c r="H90" s="21"/>
-      <c r="I90" s="60"/>
-      <c r="J90" s="60"/>
-      <c r="K90" s="60"/>
-      <c r="L90" s="60"/>
-      <c r="M90" s="60"/>
-      <c r="N90" s="61"/>
+    <row r="90" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="46"/>
+      <c r="B90" s="47"/>
+      <c r="C90" s="43"/>
+      <c r="D90" s="49"/>
+      <c r="E90" s="50"/>
+      <c r="F90" s="49"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="39"/>
+      <c r="I90" s="62"/>
+      <c r="J90" s="62"/>
+      <c r="K90" s="62"/>
+      <c r="L90" s="62"/>
+      <c r="M90" s="62"/>
+      <c r="N90" s="64"/>
       <c r="O90" s="17"/>
       <c r="P90" s="18"/>
       <c r="Q90" s="18"/>
@@ -3964,43 +4087,43 @@
       <c r="S90" s="18"/>
       <c r="T90" s="18"/>
     </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="24"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="27"/>
-      <c r="E91" s="28"/>
-      <c r="F91" s="27"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="30"/>
-      <c r="I91" s="62"/>
-      <c r="J91" s="62"/>
-      <c r="K91" s="62"/>
-      <c r="L91" s="62"/>
-      <c r="M91" s="62"/>
-      <c r="N91" s="63"/>
-      <c r="O91" s="17"/>
-      <c r="P91" s="18"/>
-      <c r="Q91" s="18"/>
-      <c r="R91" s="18"/>
-      <c r="S91" s="18"/>
-      <c r="T91" s="18"/>
-    </row>
-    <row r="92" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="24"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="41"/>
-      <c r="F92" s="37"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="30"/>
-      <c r="I92" s="62"/>
-      <c r="J92" s="62"/>
-      <c r="K92" s="62"/>
-      <c r="L92" s="62"/>
-      <c r="M92" s="62"/>
-      <c r="N92" s="64"/>
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="17" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="66"/>
+      <c r="B91" s="67"/>
+      <c r="C91" s="67"/>
+      <c r="D91" s="67"/>
+      <c r="E91" s="68"/>
+      <c r="F91" s="67"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="69"/>
+      <c r="I91" s="53"/>
+      <c r="J91" s="53"/>
+      <c r="K91" s="53"/>
+      <c r="L91" s="53"/>
+      <c r="M91" s="53"/>
+      <c r="N91" s="56"/>
+    </row>
+    <row r="92" spans="1:20" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B92" s="80"/>
+      <c r="C92" s="80"/>
+      <c r="D92" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F92" s="85"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="15"/>
+      <c r="L92" s="15"/>
+      <c r="M92" s="15"/>
+      <c r="N92" s="16"/>
       <c r="O92" s="17"/>
       <c r="P92" s="18"/>
       <c r="Q92" s="18"/>
@@ -4008,21 +4131,27 @@
       <c r="S92" s="18"/>
       <c r="T92" s="18"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="24"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="28"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="30"/>
-      <c r="I93" s="62"/>
-      <c r="J93" s="62"/>
-      <c r="K93" s="62"/>
-      <c r="L93" s="62"/>
-      <c r="M93" s="62"/>
-      <c r="N93" s="64"/>
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B93" s="83"/>
+      <c r="C93" s="83"/>
+      <c r="D93" s="70" t="s">
+        <v>84</v>
+      </c>
+      <c r="E93" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="F93" s="86"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="22"/>
+      <c r="N93" s="23"/>
       <c r="O93" s="17"/>
       <c r="P93" s="18"/>
       <c r="Q93" s="18"/>
@@ -4030,155 +4159,217 @@
       <c r="S93" s="18"/>
       <c r="T93" s="18"/>
     </row>
-    <row r="94" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="24"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="43"/>
-      <c r="D94" s="27"/>
-      <c r="E94" s="41"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="65"/>
-      <c r="J94" s="65"/>
-      <c r="K94" s="65"/>
-      <c r="L94" s="65"/>
-      <c r="M94" s="65"/>
-      <c r="N94" s="64"/>
-      <c r="O94" s="17"/>
-      <c r="P94" s="18"/>
-      <c r="Q94" s="18"/>
-      <c r="R94" s="18"/>
-      <c r="S94" s="18"/>
-      <c r="T94" s="18"/>
-    </row>
-    <row r="95" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="24"/>
-      <c r="B95" s="25"/>
-      <c r="C95" s="43"/>
-      <c r="D95" s="27"/>
-      <c r="E95" s="41"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="38"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="62"/>
-      <c r="J95" s="62"/>
-      <c r="K95" s="62"/>
-      <c r="L95" s="62"/>
-      <c r="M95" s="62"/>
-      <c r="N95" s="64"/>
-      <c r="O95" s="17"/>
-      <c r="P95" s="18"/>
-      <c r="Q95" s="18"/>
-      <c r="R95" s="18"/>
-      <c r="S95" s="18"/>
-      <c r="T95" s="18"/>
-    </row>
-    <row r="96" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="24"/>
+    <row r="94" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="24">
+        <v>1</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E94" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G94" s="29"/>
+      <c r="H94" s="30"/>
+      <c r="I94" s="31"/>
+      <c r="J94" s="31"/>
+      <c r="K94" s="31"/>
+      <c r="L94" s="31"/>
+      <c r="M94" s="31"/>
+      <c r="N94" s="32"/>
+      <c r="O94" s="33"/>
+      <c r="P94" s="34"/>
+      <c r="Q94" s="34"/>
+      <c r="R94" s="34"/>
+      <c r="S94" s="34"/>
+      <c r="T94" s="34"/>
+    </row>
+    <row r="95" spans="1:20" s="35" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="46">
+        <v>2</v>
+      </c>
+      <c r="B95" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D95" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F95" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="G95" s="29"/>
+      <c r="H95" s="30"/>
+      <c r="I95" s="31"/>
+      <c r="J95" s="31"/>
+      <c r="K95" s="31"/>
+      <c r="L95" s="31"/>
+      <c r="M95" s="31"/>
+      <c r="N95" s="32"/>
+      <c r="O95" s="33"/>
+      <c r="P95" s="34"/>
+      <c r="Q95" s="34"/>
+      <c r="R95" s="34"/>
+      <c r="S95" s="34"/>
+      <c r="T95" s="34"/>
+    </row>
+    <row r="96" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="46">
+        <v>3</v>
+      </c>
       <c r="B96" s="25"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="27"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="27"/>
-      <c r="G96" s="44"/>
+      <c r="C96" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D96" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E96" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F96" s="37"/>
+      <c r="G96" s="38"/>
       <c r="H96" s="39"/>
-      <c r="I96" s="65"/>
-      <c r="J96" s="65"/>
-      <c r="K96" s="65"/>
-      <c r="L96" s="65"/>
-      <c r="M96" s="65"/>
-      <c r="N96" s="64"/>
-      <c r="O96" s="17"/>
-      <c r="P96" s="18"/>
-      <c r="Q96" s="18"/>
-      <c r="R96" s="18"/>
-      <c r="S96" s="18"/>
-      <c r="T96" s="18"/>
-    </row>
-    <row r="97" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="24"/>
+      <c r="I96" s="31"/>
+      <c r="J96" s="31"/>
+      <c r="K96" s="31"/>
+      <c r="L96" s="31"/>
+      <c r="M96" s="31"/>
+      <c r="N96" s="40"/>
+      <c r="O96" s="33"/>
+      <c r="P96" s="34"/>
+      <c r="Q96" s="34"/>
+      <c r="R96" s="34"/>
+      <c r="S96" s="34"/>
+      <c r="T96" s="34"/>
+    </row>
+    <row r="97" spans="1:20" s="35" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="46">
+        <v>4</v>
+      </c>
       <c r="B97" s="25"/>
-      <c r="C97" s="43"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="44"/>
+      <c r="C97" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D97" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="F97" s="37"/>
+      <c r="G97" s="38"/>
       <c r="H97" s="39"/>
-      <c r="I97" s="62"/>
-      <c r="J97" s="62"/>
-      <c r="K97" s="62"/>
-      <c r="L97" s="62"/>
-      <c r="M97" s="62"/>
-      <c r="N97" s="64"/>
-      <c r="O97" s="17"/>
-      <c r="P97" s="18"/>
-      <c r="Q97" s="18"/>
-      <c r="R97" s="18"/>
-      <c r="S97" s="18"/>
-      <c r="T97" s="18"/>
-    </row>
-    <row r="98" spans="1:20" s="1" customFormat="1" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="66"/>
-      <c r="B98" s="67"/>
-      <c r="C98" s="67"/>
-      <c r="D98" s="67"/>
-      <c r="E98" s="68"/>
-      <c r="F98" s="67"/>
-      <c r="G98" s="55"/>
-      <c r="H98" s="69"/>
-      <c r="I98" s="53"/>
-      <c r="J98" s="53"/>
-      <c r="K98" s="53"/>
-      <c r="L98" s="53"/>
-      <c r="M98" s="53"/>
-      <c r="N98" s="56"/>
-    </row>
-    <row r="99" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A99" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B99" s="77"/>
-      <c r="C99" s="77"/>
-      <c r="D99" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E99" s="78" t="s">
+      <c r="I97" s="42"/>
+      <c r="J97" s="42"/>
+      <c r="K97" s="42"/>
+      <c r="L97" s="42"/>
+      <c r="M97" s="42"/>
+      <c r="N97" s="40"/>
+      <c r="O97" s="33"/>
+      <c r="P97" s="34"/>
+      <c r="Q97" s="34"/>
+      <c r="R97" s="34"/>
+      <c r="S97" s="34"/>
+      <c r="T97" s="34"/>
+    </row>
+    <row r="98" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="46">
+        <v>5</v>
+      </c>
+      <c r="B98" s="25"/>
+      <c r="C98" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D98" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" s="27"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="39"/>
+      <c r="I98" s="31"/>
+      <c r="J98" s="31"/>
+      <c r="K98" s="31"/>
+      <c r="L98" s="31"/>
+      <c r="M98" s="31"/>
+      <c r="N98" s="40"/>
+      <c r="O98" s="17"/>
+      <c r="P98" s="18"/>
+      <c r="Q98" s="18"/>
+      <c r="R98" s="18"/>
+      <c r="S98" s="18"/>
+      <c r="T98" s="18"/>
+    </row>
+    <row r="99" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="46">
         <v>6</v>
       </c>
-      <c r="F99" s="78"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="14"/>
-      <c r="I99" s="15"/>
-      <c r="J99" s="15"/>
-      <c r="K99" s="15"/>
-      <c r="L99" s="15"/>
-      <c r="M99" s="15"/>
-      <c r="N99" s="16"/>
-      <c r="O99" s="17"/>
-      <c r="P99" s="18"/>
-      <c r="Q99" s="18"/>
-      <c r="R99" s="18"/>
-      <c r="S99" s="18"/>
-      <c r="T99" s="18"/>
-    </row>
-    <row r="100" spans="1:20" s="1" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B100" s="75"/>
-      <c r="C100" s="75"/>
-      <c r="D100" s="70"/>
-      <c r="E100" s="76"/>
-      <c r="F100" s="76"/>
-      <c r="G100" s="21"/>
-      <c r="H100" s="21"/>
-      <c r="I100" s="22"/>
-      <c r="J100" s="22"/>
-      <c r="K100" s="22"/>
-      <c r="L100" s="22"/>
-      <c r="M100" s="22"/>
-      <c r="N100" s="23"/>
+      <c r="B99" s="25"/>
+      <c r="C99" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D99" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F99" s="37"/>
+      <c r="G99" s="37"/>
+      <c r="H99" s="39"/>
+      <c r="I99" s="42"/>
+      <c r="J99" s="42"/>
+      <c r="K99" s="42"/>
+      <c r="L99" s="42"/>
+      <c r="M99" s="42"/>
+      <c r="N99" s="40"/>
+      <c r="O99" s="33"/>
+      <c r="P99" s="34"/>
+      <c r="Q99" s="34"/>
+      <c r="R99" s="34"/>
+      <c r="S99" s="34"/>
+      <c r="T99" s="34"/>
+    </row>
+    <row r="100" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="46">
+        <v>7</v>
+      </c>
+      <c r="B100" s="25"/>
+      <c r="C100" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D100" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E100" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F100" s="27"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="39"/>
+      <c r="I100" s="31"/>
+      <c r="J100" s="31"/>
+      <c r="K100" s="31"/>
+      <c r="L100" s="31"/>
+      <c r="M100" s="31"/>
+      <c r="N100" s="40"/>
       <c r="O100" s="17"/>
       <c r="P100" s="18"/>
       <c r="Q100" s="18"/>
@@ -4186,27 +4377,35 @@
       <c r="S100" s="18"/>
       <c r="T100" s="18"/>
     </row>
-    <row r="101" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="24"/>
+    <row r="101" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="46">
+        <v>8</v>
+      </c>
       <c r="B101" s="25"/>
-      <c r="C101" s="26"/>
-      <c r="D101" s="27"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="38"/>
-      <c r="H101" s="30"/>
-      <c r="I101" s="62"/>
-      <c r="J101" s="62"/>
-      <c r="K101" s="62"/>
-      <c r="L101" s="62"/>
-      <c r="M101" s="62"/>
-      <c r="N101" s="63"/>
-      <c r="O101" s="17"/>
-      <c r="P101" s="18"/>
-      <c r="Q101" s="18"/>
-      <c r="R101" s="18"/>
-      <c r="S101" s="18"/>
-      <c r="T101" s="18"/>
+      <c r="C101" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D101" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E101" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F101" s="27"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="39"/>
+      <c r="I101" s="42"/>
+      <c r="J101" s="42"/>
+      <c r="K101" s="42"/>
+      <c r="L101" s="42"/>
+      <c r="M101" s="42"/>
+      <c r="N101" s="40"/>
+      <c r="O101" s="33"/>
+      <c r="P101" s="34"/>
+      <c r="Q101" s="34"/>
+      <c r="R101" s="34"/>
+      <c r="S101" s="34"/>
+      <c r="T101" s="34"/>
     </row>
     <row r="102" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A102" s="24"/>
@@ -4230,43 +4429,43 @@
       <c r="S102" s="18"/>
       <c r="T102" s="18"/>
     </row>
-    <row r="103" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="24"/>
-      <c r="B103" s="25"/>
-      <c r="C103" s="26"/>
-      <c r="D103" s="27"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="37"/>
-      <c r="G103" s="38"/>
-      <c r="H103" s="30"/>
-      <c r="I103" s="62"/>
-      <c r="J103" s="62"/>
-      <c r="K103" s="62"/>
-      <c r="L103" s="62"/>
-      <c r="M103" s="62"/>
-      <c r="N103" s="63"/>
-      <c r="O103" s="17"/>
-      <c r="P103" s="18"/>
-      <c r="Q103" s="18"/>
-      <c r="R103" s="18"/>
-      <c r="S103" s="18"/>
-      <c r="T103" s="18"/>
-    </row>
-    <row r="104" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="24"/>
-      <c r="B104" s="25"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="27"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="37"/>
-      <c r="G104" s="38"/>
-      <c r="H104" s="30"/>
-      <c r="I104" s="62"/>
-      <c r="J104" s="62"/>
-      <c r="K104" s="62"/>
-      <c r="L104" s="62"/>
-      <c r="M104" s="62"/>
-      <c r="N104" s="63"/>
+    <row r="103" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="66"/>
+      <c r="B103" s="67"/>
+      <c r="C103" s="67"/>
+      <c r="D103" s="67"/>
+      <c r="E103" s="68"/>
+      <c r="F103" s="67"/>
+      <c r="G103" s="67"/>
+      <c r="H103" s="67"/>
+      <c r="I103" s="67"/>
+      <c r="J103" s="67"/>
+      <c r="K103" s="67"/>
+      <c r="L103" s="67"/>
+      <c r="M103" s="67"/>
+      <c r="N103" s="71"/>
+    </row>
+    <row r="104" spans="1:20" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B104" s="80"/>
+      <c r="C104" s="80"/>
+      <c r="D104" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E104" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F104" s="85"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
+      <c r="L104" s="15"/>
+      <c r="M104" s="15"/>
+      <c r="N104" s="16"/>
       <c r="O104" s="17"/>
       <c r="P104" s="18"/>
       <c r="Q104" s="18"/>
@@ -4274,21 +4473,27 @@
       <c r="S104" s="18"/>
       <c r="T104" s="18"/>
     </row>
-    <row r="105" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="24"/>
-      <c r="B105" s="25"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="36"/>
-      <c r="F105" s="37"/>
-      <c r="G105" s="38"/>
-      <c r="H105" s="30"/>
-      <c r="I105" s="62"/>
-      <c r="J105" s="62"/>
-      <c r="K105" s="62"/>
-      <c r="L105" s="62"/>
-      <c r="M105" s="62"/>
-      <c r="N105" s="63"/>
+    <row r="105" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B105" s="83"/>
+      <c r="C105" s="83"/>
+      <c r="D105" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E105" s="86" t="s">
+        <v>104</v>
+      </c>
+      <c r="F105" s="86"/>
+      <c r="G105" s="73"/>
+      <c r="H105" s="73"/>
+      <c r="I105" s="22"/>
+      <c r="J105" s="22"/>
+      <c r="K105" s="22"/>
+      <c r="L105" s="22"/>
+      <c r="M105" s="22"/>
+      <c r="N105" s="23"/>
       <c r="O105" s="17"/>
       <c r="P105" s="18"/>
       <c r="Q105" s="18"/>
@@ -4296,133 +4501,185 @@
       <c r="S105" s="18"/>
       <c r="T105" s="18"/>
     </row>
-    <row r="106" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="66"/>
-      <c r="B106" s="67"/>
-      <c r="C106" s="67"/>
-      <c r="D106" s="67"/>
-      <c r="E106" s="68"/>
-      <c r="F106" s="67"/>
-      <c r="G106" s="67"/>
-      <c r="H106" s="67"/>
-      <c r="I106" s="67"/>
-      <c r="J106" s="67"/>
-      <c r="K106" s="67"/>
-      <c r="L106" s="67"/>
-      <c r="M106" s="67"/>
-      <c r="N106" s="71"/>
-    </row>
-    <row r="107" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A107" s="77" t="s">
-        <v>16</v>
-      </c>
-      <c r="B107" s="77"/>
-      <c r="C107" s="77"/>
-      <c r="D107" s="57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E107" s="78" t="s">
+    <row r="106" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="46">
+        <v>1</v>
+      </c>
+      <c r="B106" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D106" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E106" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="F106" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" s="29"/>
+      <c r="H106" s="30"/>
+      <c r="I106" s="31"/>
+      <c r="J106" s="31"/>
+      <c r="K106" s="31"/>
+      <c r="L106" s="31"/>
+      <c r="M106" s="31"/>
+      <c r="N106" s="32"/>
+      <c r="O106" s="33"/>
+      <c r="P106" s="34"/>
+      <c r="Q106" s="34"/>
+      <c r="R106" s="34"/>
+      <c r="S106" s="34"/>
+      <c r="T106" s="34"/>
+    </row>
+    <row r="107" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="46">
+        <v>2</v>
+      </c>
+      <c r="B107" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C107" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="D107" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E107" s="50"/>
+      <c r="F107" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="G107" s="29"/>
+      <c r="H107" s="30"/>
+      <c r="I107" s="31"/>
+      <c r="J107" s="31"/>
+      <c r="K107" s="31"/>
+      <c r="L107" s="31"/>
+      <c r="M107" s="31"/>
+      <c r="N107" s="32"/>
+      <c r="O107" s="33"/>
+      <c r="P107" s="34"/>
+      <c r="Q107" s="34"/>
+      <c r="R107" s="34"/>
+      <c r="S107" s="34"/>
+      <c r="T107" s="34"/>
+    </row>
+    <row r="108" spans="1:20" s="35" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="46">
+        <v>3</v>
+      </c>
+      <c r="B108" s="47"/>
+      <c r="C108" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="D108" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E108" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="F108" s="51"/>
+      <c r="G108" s="29"/>
+      <c r="H108" s="30"/>
+      <c r="I108" s="31"/>
+      <c r="J108" s="31"/>
+      <c r="K108" s="31"/>
+      <c r="L108" s="31"/>
+      <c r="M108" s="31"/>
+      <c r="N108" s="32"/>
+      <c r="O108" s="33"/>
+      <c r="P108" s="34"/>
+      <c r="Q108" s="34"/>
+      <c r="R108" s="34"/>
+      <c r="S108" s="34"/>
+      <c r="T108" s="34"/>
+    </row>
+    <row r="109" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="46">
+        <v>4</v>
+      </c>
+      <c r="B109" s="47"/>
+      <c r="C109" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D109" s="76" t="s">
+        <v>90</v>
+      </c>
+      <c r="E109" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F109" s="51"/>
+      <c r="G109" s="38"/>
+      <c r="H109" s="39"/>
+      <c r="I109" s="31"/>
+      <c r="J109" s="31"/>
+      <c r="K109" s="31"/>
+      <c r="L109" s="31"/>
+      <c r="M109" s="31"/>
+      <c r="N109" s="40"/>
+      <c r="O109" s="33"/>
+      <c r="P109" s="34"/>
+      <c r="Q109" s="34"/>
+      <c r="R109" s="34"/>
+      <c r="S109" s="34"/>
+      <c r="T109" s="34"/>
+    </row>
+    <row r="110" spans="1:20" s="35" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="46">
+        <v>5</v>
+      </c>
+      <c r="B110" s="47"/>
+      <c r="C110" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="D110" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E110" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="F110" s="51"/>
+      <c r="G110" s="38"/>
+      <c r="H110" s="39"/>
+      <c r="I110" s="42"/>
+      <c r="J110" s="42"/>
+      <c r="K110" s="42"/>
+      <c r="L110" s="42"/>
+      <c r="M110" s="42"/>
+      <c r="N110" s="40"/>
+      <c r="O110" s="33"/>
+      <c r="P110" s="34"/>
+      <c r="Q110" s="34"/>
+      <c r="R110" s="34"/>
+      <c r="S110" s="34"/>
+      <c r="T110" s="34"/>
+    </row>
+    <row r="111" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="46">
         <v>6</v>
       </c>
-      <c r="F107" s="78"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="14"/>
-      <c r="I107" s="15"/>
-      <c r="J107" s="15"/>
-      <c r="K107" s="15"/>
-      <c r="L107" s="15"/>
-      <c r="M107" s="15"/>
-      <c r="N107" s="16"/>
-      <c r="O107" s="17"/>
-      <c r="P107" s="18"/>
-      <c r="Q107" s="18"/>
-      <c r="R107" s="18"/>
-      <c r="S107" s="18"/>
-      <c r="T107" s="18"/>
-    </row>
-    <row r="108" spans="1:20" s="1" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B108" s="75"/>
-      <c r="C108" s="75"/>
-      <c r="D108" s="70"/>
-      <c r="E108" s="76"/>
-      <c r="F108" s="76"/>
-      <c r="G108" s="21"/>
-      <c r="H108" s="21"/>
-      <c r="I108" s="22"/>
-      <c r="J108" s="22"/>
-      <c r="K108" s="22"/>
-      <c r="L108" s="22"/>
-      <c r="M108" s="22"/>
-      <c r="N108" s="23"/>
-      <c r="O108" s="17"/>
-      <c r="P108" s="18"/>
-      <c r="Q108" s="18"/>
-      <c r="R108" s="18"/>
-      <c r="S108" s="18"/>
-      <c r="T108" s="18"/>
-    </row>
-    <row r="109" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="24"/>
-      <c r="B109" s="25"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="27"/>
-      <c r="E109" s="36"/>
-      <c r="F109" s="37"/>
-      <c r="G109" s="38"/>
-      <c r="H109" s="30"/>
-      <c r="I109" s="62"/>
-      <c r="J109" s="62"/>
-      <c r="K109" s="62"/>
-      <c r="L109" s="62"/>
-      <c r="M109" s="62"/>
-      <c r="N109" s="63"/>
-      <c r="O109" s="17"/>
-      <c r="P109" s="18"/>
-      <c r="Q109" s="18"/>
-      <c r="R109" s="18"/>
-      <c r="S109" s="18"/>
-      <c r="T109" s="18"/>
-    </row>
-    <row r="110" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="24"/>
-      <c r="B110" s="25"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="27"/>
-      <c r="E110" s="36"/>
-      <c r="F110" s="37"/>
-      <c r="G110" s="38"/>
-      <c r="H110" s="30"/>
-      <c r="I110" s="62"/>
-      <c r="J110" s="62"/>
-      <c r="K110" s="62"/>
-      <c r="L110" s="62"/>
-      <c r="M110" s="62"/>
-      <c r="N110" s="63"/>
-      <c r="O110" s="17"/>
-      <c r="P110" s="18"/>
-      <c r="Q110" s="18"/>
-      <c r="R110" s="18"/>
-      <c r="S110" s="18"/>
-      <c r="T110" s="18"/>
-    </row>
-    <row r="111" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="24"/>
-      <c r="B111" s="25"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="36"/>
-      <c r="F111" s="37"/>
-      <c r="G111" s="38"/>
-      <c r="H111" s="30"/>
-      <c r="I111" s="62"/>
-      <c r="J111" s="62"/>
-      <c r="K111" s="62"/>
-      <c r="L111" s="62"/>
-      <c r="M111" s="62"/>
-      <c r="N111" s="63"/>
+      <c r="B111" s="47"/>
+      <c r="C111" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D111" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E111" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F111" s="49"/>
+      <c r="G111" s="51"/>
+      <c r="H111" s="39"/>
+      <c r="I111" s="31"/>
+      <c r="J111" s="31"/>
+      <c r="K111" s="31"/>
+      <c r="L111" s="31"/>
+      <c r="M111" s="31"/>
+      <c r="N111" s="40"/>
       <c r="O111" s="17"/>
       <c r="P111" s="18"/>
       <c r="Q111" s="18"/>
@@ -4430,43 +4687,59 @@
       <c r="S111" s="18"/>
       <c r="T111" s="18"/>
     </row>
-    <row r="112" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="24"/>
-      <c r="B112" s="25"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="36"/>
-      <c r="F112" s="37"/>
-      <c r="G112" s="38"/>
-      <c r="H112" s="30"/>
-      <c r="I112" s="62"/>
-      <c r="J112" s="62"/>
-      <c r="K112" s="62"/>
-      <c r="L112" s="62"/>
-      <c r="M112" s="62"/>
-      <c r="N112" s="63"/>
-      <c r="O112" s="17"/>
-      <c r="P112" s="18"/>
-      <c r="Q112" s="18"/>
-      <c r="R112" s="18"/>
-      <c r="S112" s="18"/>
-      <c r="T112" s="18"/>
-    </row>
-    <row r="113" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="24"/>
-      <c r="B113" s="25"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="36"/>
-      <c r="F113" s="37"/>
-      <c r="G113" s="38"/>
-      <c r="H113" s="30"/>
-      <c r="I113" s="62"/>
-      <c r="J113" s="62"/>
-      <c r="K113" s="62"/>
-      <c r="L113" s="62"/>
-      <c r="M113" s="62"/>
-      <c r="N113" s="63"/>
+    <row r="112" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="46">
+        <v>7</v>
+      </c>
+      <c r="B112" s="47"/>
+      <c r="C112" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D112" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E112" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F112" s="51"/>
+      <c r="G112" s="51"/>
+      <c r="H112" s="39"/>
+      <c r="I112" s="42"/>
+      <c r="J112" s="42"/>
+      <c r="K112" s="42"/>
+      <c r="L112" s="42"/>
+      <c r="M112" s="42"/>
+      <c r="N112" s="40"/>
+      <c r="O112" s="33"/>
+      <c r="P112" s="34"/>
+      <c r="Q112" s="34"/>
+      <c r="R112" s="34"/>
+      <c r="S112" s="34"/>
+      <c r="T112" s="34"/>
+    </row>
+    <row r="113" spans="1:20" s="1" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="46">
+        <v>8</v>
+      </c>
+      <c r="B113" s="47"/>
+      <c r="C113" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D113" s="49" t="s">
+        <v>55</v>
+      </c>
+      <c r="E113" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F113" s="49"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="39"/>
+      <c r="I113" s="31"/>
+      <c r="J113" s="31"/>
+      <c r="K113" s="31"/>
+      <c r="L113" s="31"/>
+      <c r="M113" s="31"/>
+      <c r="N113" s="40"/>
       <c r="O113" s="17"/>
       <c r="P113" s="18"/>
       <c r="Q113" s="18"/>
@@ -4474,110 +4747,648 @@
       <c r="S113" s="18"/>
       <c r="T113" s="18"/>
     </row>
-    <row r="114" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="66"/>
-      <c r="B114" s="67"/>
-      <c r="C114" s="67"/>
-      <c r="D114" s="67"/>
-      <c r="E114" s="68"/>
-      <c r="F114" s="67"/>
-      <c r="G114" s="67"/>
-      <c r="H114" s="67"/>
-      <c r="I114" s="67"/>
-      <c r="J114" s="67"/>
-      <c r="K114" s="67"/>
-      <c r="L114" s="67"/>
-      <c r="M114" s="67"/>
-      <c r="N114" s="71"/>
-    </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E115" s="72"/>
-    </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E116" s="72"/>
-    </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E117" s="72"/>
-    </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E118" s="72"/>
-    </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E119" s="72"/>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E120" s="72"/>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E121" s="72"/>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E122" s="72"/>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E123" s="72"/>
-    </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E124" s="72"/>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E125" s="72"/>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E126" s="72"/>
-    </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E127" s="72"/>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="E128" s="72"/>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E129" s="72"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E130" s="72"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E131" s="72"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E132" s="72"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E133" s="72"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E134" s="72"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E135" s="72"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E136" s="72"/>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E137" s="72"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E138" s="72"/>
-    </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E139" s="72"/>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E140" s="72"/>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E141" s="72"/>
-    </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E142" s="72"/>
-    </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:20" s="35" customFormat="1" ht="28" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="46">
+        <v>9</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D114" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E114" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="F114" s="49"/>
+      <c r="G114" s="44"/>
+      <c r="H114" s="39"/>
+      <c r="I114" s="42"/>
+      <c r="J114" s="42"/>
+      <c r="K114" s="42"/>
+      <c r="L114" s="42"/>
+      <c r="M114" s="42"/>
+      <c r="N114" s="40"/>
+      <c r="O114" s="33"/>
+      <c r="P114" s="34"/>
+      <c r="Q114" s="34"/>
+      <c r="R114" s="34"/>
+      <c r="S114" s="34"/>
+      <c r="T114" s="34"/>
+    </row>
+    <row r="115" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="46"/>
+      <c r="B115" s="47"/>
+      <c r="C115" s="48"/>
+      <c r="D115" s="49"/>
+      <c r="E115" s="36"/>
+      <c r="F115" s="51"/>
+      <c r="G115" s="38"/>
+      <c r="H115" s="30"/>
+      <c r="I115" s="62"/>
+      <c r="J115" s="62"/>
+      <c r="K115" s="62"/>
+      <c r="L115" s="62"/>
+      <c r="M115" s="62"/>
+      <c r="N115" s="63"/>
+      <c r="O115" s="17"/>
+      <c r="P115" s="18"/>
+      <c r="Q115" s="18"/>
+      <c r="R115" s="18"/>
+      <c r="S115" s="18"/>
+      <c r="T115" s="18"/>
+    </row>
+    <row r="116" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="66"/>
+      <c r="B116" s="67"/>
+      <c r="C116" s="67"/>
+      <c r="D116" s="67"/>
+      <c r="E116" s="68"/>
+      <c r="F116" s="67"/>
+      <c r="G116" s="67"/>
+      <c r="H116" s="67"/>
+      <c r="I116" s="67"/>
+      <c r="J116" s="67"/>
+      <c r="K116" s="67"/>
+      <c r="L116" s="67"/>
+      <c r="M116" s="67"/>
+      <c r="N116" s="71"/>
+    </row>
+    <row r="117" spans="1:20" s="1" customFormat="1" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="80"/>
+      <c r="B117" s="80"/>
+      <c r="C117" s="80"/>
+      <c r="D117" s="57"/>
+      <c r="E117" s="81"/>
+      <c r="F117" s="81"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="15"/>
+      <c r="J117" s="15"/>
+      <c r="K117" s="15"/>
+      <c r="L117" s="15"/>
+      <c r="M117" s="15"/>
+      <c r="N117" s="16"/>
+      <c r="O117" s="17"/>
+      <c r="P117" s="18"/>
+      <c r="Q117" s="18"/>
+      <c r="R117" s="18"/>
+      <c r="S117" s="18"/>
+      <c r="T117" s="18"/>
+    </row>
+    <row r="118" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A118" s="83"/>
+      <c r="B118" s="83"/>
+      <c r="C118" s="83"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="84"/>
+      <c r="F118" s="84"/>
+      <c r="G118" s="21"/>
+      <c r="H118" s="21"/>
+      <c r="I118" s="60"/>
+      <c r="J118" s="60"/>
+      <c r="K118" s="60"/>
+      <c r="L118" s="60"/>
+      <c r="M118" s="60"/>
+      <c r="N118" s="61"/>
+      <c r="O118" s="17"/>
+      <c r="P118" s="18"/>
+      <c r="Q118" s="18"/>
+      <c r="R118" s="18"/>
+      <c r="S118" s="18"/>
+      <c r="T118" s="18"/>
+    </row>
+    <row r="119" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="24"/>
+      <c r="B119" s="25"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="28"/>
+      <c r="F119" s="27"/>
+      <c r="G119" s="38"/>
+      <c r="H119" s="30"/>
+      <c r="I119" s="62"/>
+      <c r="J119" s="62"/>
+      <c r="K119" s="62"/>
+      <c r="L119" s="62"/>
+      <c r="M119" s="62"/>
+      <c r="N119" s="63"/>
+      <c r="O119" s="17"/>
+      <c r="P119" s="18"/>
+      <c r="Q119" s="18"/>
+      <c r="R119" s="18"/>
+      <c r="S119" s="18"/>
+      <c r="T119" s="18"/>
+    </row>
+    <row r="120" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="24"/>
+      <c r="B120" s="25"/>
+      <c r="C120" s="26"/>
+      <c r="D120" s="27"/>
+      <c r="E120" s="41"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="38"/>
+      <c r="H120" s="30"/>
+      <c r="I120" s="62"/>
+      <c r="J120" s="62"/>
+      <c r="K120" s="62"/>
+      <c r="L120" s="62"/>
+      <c r="M120" s="62"/>
+      <c r="N120" s="64"/>
+      <c r="O120" s="17"/>
+      <c r="P120" s="18"/>
+      <c r="Q120" s="18"/>
+      <c r="R120" s="18"/>
+      <c r="S120" s="18"/>
+      <c r="T120" s="18"/>
+    </row>
+    <row r="121" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="24"/>
+      <c r="B121" s="25"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="38"/>
+      <c r="H121" s="30"/>
+      <c r="I121" s="62"/>
+      <c r="J121" s="62"/>
+      <c r="K121" s="62"/>
+      <c r="L121" s="62"/>
+      <c r="M121" s="62"/>
+      <c r="N121" s="64"/>
+      <c r="O121" s="17"/>
+      <c r="P121" s="18"/>
+      <c r="Q121" s="18"/>
+      <c r="R121" s="18"/>
+      <c r="S121" s="18"/>
+      <c r="T121" s="18"/>
+    </row>
+    <row r="122" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="24"/>
+      <c r="B122" s="25"/>
+      <c r="C122" s="43"/>
+      <c r="D122" s="27"/>
+      <c r="E122" s="41"/>
+      <c r="F122" s="27"/>
+      <c r="G122" s="38"/>
+      <c r="H122" s="39"/>
+      <c r="I122" s="65"/>
+      <c r="J122" s="65"/>
+      <c r="K122" s="65"/>
+      <c r="L122" s="65"/>
+      <c r="M122" s="65"/>
+      <c r="N122" s="64"/>
+      <c r="O122" s="17"/>
+      <c r="P122" s="18"/>
+      <c r="Q122" s="18"/>
+      <c r="R122" s="18"/>
+      <c r="S122" s="18"/>
+      <c r="T122" s="18"/>
+    </row>
+    <row r="123" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="24"/>
+      <c r="B123" s="25"/>
+      <c r="C123" s="43"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="41"/>
+      <c r="F123" s="27"/>
+      <c r="G123" s="38"/>
+      <c r="H123" s="39"/>
+      <c r="I123" s="62"/>
+      <c r="J123" s="62"/>
+      <c r="K123" s="62"/>
+      <c r="L123" s="62"/>
+      <c r="M123" s="62"/>
+      <c r="N123" s="64"/>
+      <c r="O123" s="17"/>
+      <c r="P123" s="18"/>
+      <c r="Q123" s="18"/>
+      <c r="R123" s="18"/>
+      <c r="S123" s="18"/>
+      <c r="T123" s="18"/>
+    </row>
+    <row r="124" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="24"/>
+      <c r="B124" s="25"/>
+      <c r="C124" s="26"/>
+      <c r="D124" s="27"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="27"/>
+      <c r="G124" s="44"/>
+      <c r="H124" s="39"/>
+      <c r="I124" s="65"/>
+      <c r="J124" s="65"/>
+      <c r="K124" s="65"/>
+      <c r="L124" s="65"/>
+      <c r="M124" s="65"/>
+      <c r="N124" s="64"/>
+      <c r="O124" s="17"/>
+      <c r="P124" s="18"/>
+      <c r="Q124" s="18"/>
+      <c r="R124" s="18"/>
+      <c r="S124" s="18"/>
+      <c r="T124" s="18"/>
+    </row>
+    <row r="125" spans="1:20" s="1" customFormat="1" ht="20" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="24"/>
+      <c r="B125" s="25"/>
+      <c r="C125" s="43"/>
+      <c r="D125" s="27"/>
+      <c r="E125" s="28"/>
+      <c r="F125" s="27"/>
+      <c r="G125" s="44"/>
+      <c r="H125" s="39"/>
+      <c r="I125" s="62"/>
+      <c r="J125" s="62"/>
+      <c r="K125" s="62"/>
+      <c r="L125" s="62"/>
+      <c r="M125" s="62"/>
+      <c r="N125" s="64"/>
+      <c r="O125" s="17"/>
+      <c r="P125" s="18"/>
+      <c r="Q125" s="18"/>
+      <c r="R125" s="18"/>
+      <c r="S125" s="18"/>
+      <c r="T125" s="18"/>
+    </row>
+    <row r="126" spans="1:20" s="1" customFormat="1" ht="16" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="66"/>
+      <c r="B126" s="67"/>
+      <c r="C126" s="67"/>
+      <c r="D126" s="67"/>
+      <c r="E126" s="68"/>
+      <c r="F126" s="67"/>
+      <c r="G126" s="55"/>
+      <c r="H126" s="69"/>
+      <c r="I126" s="53"/>
+      <c r="J126" s="53"/>
+      <c r="K126" s="53"/>
+      <c r="L126" s="53"/>
+      <c r="M126" s="53"/>
+      <c r="N126" s="56"/>
+    </row>
+    <row r="127" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A127" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B127" s="80"/>
+      <c r="C127" s="80"/>
+      <c r="D127" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F127" s="85"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="14"/>
+      <c r="I127" s="15"/>
+      <c r="J127" s="15"/>
+      <c r="K127" s="15"/>
+      <c r="L127" s="15"/>
+      <c r="M127" s="15"/>
+      <c r="N127" s="16"/>
+      <c r="O127" s="17"/>
+      <c r="P127" s="18"/>
+      <c r="Q127" s="18"/>
+      <c r="R127" s="18"/>
+      <c r="S127" s="18"/>
+      <c r="T127" s="18"/>
+    </row>
+    <row r="128" spans="1:20" s="1" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B128" s="87"/>
+      <c r="C128" s="87"/>
+      <c r="D128" s="70"/>
+      <c r="E128" s="86"/>
+      <c r="F128" s="86"/>
+      <c r="G128" s="21"/>
+      <c r="H128" s="21"/>
+      <c r="I128" s="22"/>
+      <c r="J128" s="22"/>
+      <c r="K128" s="22"/>
+      <c r="L128" s="22"/>
+      <c r="M128" s="22"/>
+      <c r="N128" s="23"/>
+      <c r="O128" s="17"/>
+      <c r="P128" s="18"/>
+      <c r="Q128" s="18"/>
+      <c r="R128" s="18"/>
+      <c r="S128" s="18"/>
+      <c r="T128" s="18"/>
+    </row>
+    <row r="129" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="24"/>
+      <c r="B129" s="25"/>
+      <c r="C129" s="26"/>
+      <c r="D129" s="27"/>
+      <c r="E129" s="36"/>
+      <c r="F129" s="37"/>
+      <c r="G129" s="38"/>
+      <c r="H129" s="30"/>
+      <c r="I129" s="62"/>
+      <c r="J129" s="62"/>
+      <c r="K129" s="62"/>
+      <c r="L129" s="62"/>
+      <c r="M129" s="62"/>
+      <c r="N129" s="63"/>
+      <c r="O129" s="17"/>
+      <c r="P129" s="18"/>
+      <c r="Q129" s="18"/>
+      <c r="R129" s="18"/>
+      <c r="S129" s="18"/>
+      <c r="T129" s="18"/>
+    </row>
+    <row r="130" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="24"/>
+      <c r="B130" s="25"/>
+      <c r="C130" s="26"/>
+      <c r="D130" s="27"/>
+      <c r="E130" s="36"/>
+      <c r="F130" s="37"/>
+      <c r="G130" s="38"/>
+      <c r="H130" s="30"/>
+      <c r="I130" s="62"/>
+      <c r="J130" s="62"/>
+      <c r="K130" s="62"/>
+      <c r="L130" s="62"/>
+      <c r="M130" s="62"/>
+      <c r="N130" s="63"/>
+      <c r="O130" s="17"/>
+      <c r="P130" s="18"/>
+      <c r="Q130" s="18"/>
+      <c r="R130" s="18"/>
+      <c r="S130" s="18"/>
+      <c r="T130" s="18"/>
+    </row>
+    <row r="131" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="24"/>
+      <c r="B131" s="25"/>
+      <c r="C131" s="26"/>
+      <c r="D131" s="27"/>
+      <c r="E131" s="36"/>
+      <c r="F131" s="37"/>
+      <c r="G131" s="38"/>
+      <c r="H131" s="30"/>
+      <c r="I131" s="62"/>
+      <c r="J131" s="62"/>
+      <c r="K131" s="62"/>
+      <c r="L131" s="62"/>
+      <c r="M131" s="62"/>
+      <c r="N131" s="63"/>
+      <c r="O131" s="17"/>
+      <c r="P131" s="18"/>
+      <c r="Q131" s="18"/>
+      <c r="R131" s="18"/>
+      <c r="S131" s="18"/>
+      <c r="T131" s="18"/>
+    </row>
+    <row r="132" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="24"/>
+      <c r="B132" s="25"/>
+      <c r="C132" s="26"/>
+      <c r="D132" s="27"/>
+      <c r="E132" s="36"/>
+      <c r="F132" s="37"/>
+      <c r="G132" s="38"/>
+      <c r="H132" s="30"/>
+      <c r="I132" s="62"/>
+      <c r="J132" s="62"/>
+      <c r="K132" s="62"/>
+      <c r="L132" s="62"/>
+      <c r="M132" s="62"/>
+      <c r="N132" s="63"/>
+      <c r="O132" s="17"/>
+      <c r="P132" s="18"/>
+      <c r="Q132" s="18"/>
+      <c r="R132" s="18"/>
+      <c r="S132" s="18"/>
+      <c r="T132" s="18"/>
+    </row>
+    <row r="133" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="24"/>
+      <c r="B133" s="25"/>
+      <c r="C133" s="26"/>
+      <c r="D133" s="27"/>
+      <c r="E133" s="36"/>
+      <c r="F133" s="37"/>
+      <c r="G133" s="38"/>
+      <c r="H133" s="30"/>
+      <c r="I133" s="62"/>
+      <c r="J133" s="62"/>
+      <c r="K133" s="62"/>
+      <c r="L133" s="62"/>
+      <c r="M133" s="62"/>
+      <c r="N133" s="63"/>
+      <c r="O133" s="17"/>
+      <c r="P133" s="18"/>
+      <c r="Q133" s="18"/>
+      <c r="R133" s="18"/>
+      <c r="S133" s="18"/>
+      <c r="T133" s="18"/>
+    </row>
+    <row r="134" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="66"/>
+      <c r="B134" s="67"/>
+      <c r="C134" s="67"/>
+      <c r="D134" s="67"/>
+      <c r="E134" s="68"/>
+      <c r="F134" s="67"/>
+      <c r="G134" s="67"/>
+      <c r="H134" s="67"/>
+      <c r="I134" s="67"/>
+      <c r="J134" s="67"/>
+      <c r="K134" s="67"/>
+      <c r="L134" s="67"/>
+      <c r="M134" s="67"/>
+      <c r="N134" s="71"/>
+    </row>
+    <row r="135" spans="1:20" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A135" s="80" t="s">
+        <v>16</v>
+      </c>
+      <c r="B135" s="80"/>
+      <c r="C135" s="80"/>
+      <c r="D135" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E135" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F135" s="85"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="14"/>
+      <c r="I135" s="15"/>
+      <c r="J135" s="15"/>
+      <c r="K135" s="15"/>
+      <c r="L135" s="15"/>
+      <c r="M135" s="15"/>
+      <c r="N135" s="16"/>
+      <c r="O135" s="17"/>
+      <c r="P135" s="18"/>
+      <c r="Q135" s="18"/>
+      <c r="R135" s="18"/>
+      <c r="S135" s="18"/>
+      <c r="T135" s="18"/>
+    </row>
+    <row r="136" spans="1:20" s="1" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" s="87"/>
+      <c r="C136" s="87"/>
+      <c r="D136" s="70"/>
+      <c r="E136" s="86"/>
+      <c r="F136" s="86"/>
+      <c r="G136" s="21"/>
+      <c r="H136" s="21"/>
+      <c r="I136" s="22"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="22"/>
+      <c r="L136" s="22"/>
+      <c r="M136" s="22"/>
+      <c r="N136" s="23"/>
+      <c r="O136" s="17"/>
+      <c r="P136" s="18"/>
+      <c r="Q136" s="18"/>
+      <c r="R136" s="18"/>
+      <c r="S136" s="18"/>
+      <c r="T136" s="18"/>
+    </row>
+    <row r="137" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="24"/>
+      <c r="B137" s="25"/>
+      <c r="C137" s="26"/>
+      <c r="D137" s="27"/>
+      <c r="E137" s="36"/>
+      <c r="F137" s="37"/>
+      <c r="G137" s="38"/>
+      <c r="H137" s="30"/>
+      <c r="I137" s="62"/>
+      <c r="J137" s="62"/>
+      <c r="K137" s="62"/>
+      <c r="L137" s="62"/>
+      <c r="M137" s="62"/>
+      <c r="N137" s="63"/>
+      <c r="O137" s="17"/>
+      <c r="P137" s="18"/>
+      <c r="Q137" s="18"/>
+      <c r="R137" s="18"/>
+      <c r="S137" s="18"/>
+      <c r="T137" s="18"/>
+    </row>
+    <row r="138" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="24"/>
+      <c r="B138" s="25"/>
+      <c r="C138" s="26"/>
+      <c r="D138" s="27"/>
+      <c r="E138" s="36"/>
+      <c r="F138" s="37"/>
+      <c r="G138" s="38"/>
+      <c r="H138" s="30"/>
+      <c r="I138" s="62"/>
+      <c r="J138" s="62"/>
+      <c r="K138" s="62"/>
+      <c r="L138" s="62"/>
+      <c r="M138" s="62"/>
+      <c r="N138" s="63"/>
+      <c r="O138" s="17"/>
+      <c r="P138" s="18"/>
+      <c r="Q138" s="18"/>
+      <c r="R138" s="18"/>
+      <c r="S138" s="18"/>
+      <c r="T138" s="18"/>
+    </row>
+    <row r="139" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="24"/>
+      <c r="B139" s="25"/>
+      <c r="C139" s="26"/>
+      <c r="D139" s="27"/>
+      <c r="E139" s="36"/>
+      <c r="F139" s="37"/>
+      <c r="G139" s="38"/>
+      <c r="H139" s="30"/>
+      <c r="I139" s="62"/>
+      <c r="J139" s="62"/>
+      <c r="K139" s="62"/>
+      <c r="L139" s="62"/>
+      <c r="M139" s="62"/>
+      <c r="N139" s="63"/>
+      <c r="O139" s="17"/>
+      <c r="P139" s="18"/>
+      <c r="Q139" s="18"/>
+      <c r="R139" s="18"/>
+      <c r="S139" s="18"/>
+      <c r="T139" s="18"/>
+    </row>
+    <row r="140" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="24"/>
+      <c r="B140" s="25"/>
+      <c r="C140" s="26"/>
+      <c r="D140" s="27"/>
+      <c r="E140" s="36"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="38"/>
+      <c r="H140" s="30"/>
+      <c r="I140" s="62"/>
+      <c r="J140" s="62"/>
+      <c r="K140" s="62"/>
+      <c r="L140" s="62"/>
+      <c r="M140" s="62"/>
+      <c r="N140" s="63"/>
+      <c r="O140" s="17"/>
+      <c r="P140" s="18"/>
+      <c r="Q140" s="18"/>
+      <c r="R140" s="18"/>
+      <c r="S140" s="18"/>
+      <c r="T140" s="18"/>
+    </row>
+    <row r="141" spans="1:20" s="1" customFormat="1" ht="28" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="24"/>
+      <c r="B141" s="25"/>
+      <c r="C141" s="26"/>
+      <c r="D141" s="27"/>
+      <c r="E141" s="36"/>
+      <c r="F141" s="37"/>
+      <c r="G141" s="38"/>
+      <c r="H141" s="30"/>
+      <c r="I141" s="62"/>
+      <c r="J141" s="62"/>
+      <c r="K141" s="62"/>
+      <c r="L141" s="62"/>
+      <c r="M141" s="62"/>
+      <c r="N141" s="63"/>
+      <c r="O141" s="17"/>
+      <c r="P141" s="18"/>
+      <c r="Q141" s="18"/>
+      <c r="R141" s="18"/>
+      <c r="S141" s="18"/>
+      <c r="T141" s="18"/>
+    </row>
+    <row r="142" spans="1:20" s="35" customFormat="1" ht="31" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="66"/>
+      <c r="B142" s="67"/>
+      <c r="C142" s="67"/>
+      <c r="D142" s="67"/>
+      <c r="E142" s="68"/>
+      <c r="F142" s="67"/>
+      <c r="G142" s="67"/>
+      <c r="H142" s="67"/>
+      <c r="I142" s="67"/>
+      <c r="J142" s="67"/>
+      <c r="K142" s="67"/>
+      <c r="L142" s="67"/>
+      <c r="M142" s="67"/>
+      <c r="N142" s="71"/>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.15">
       <c r="E143" s="72"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.15">
       <c r="E144" s="72"/>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.15">
@@ -7196,42 +8007,134 @@
     <row r="1016" spans="5:5" x14ac:dyDescent="0.15">
       <c r="E1016" s="72"/>
     </row>
+    <row r="1017" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1017" s="72"/>
+    </row>
+    <row r="1018" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1018" s="72"/>
+    </row>
+    <row r="1019" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1019" s="72"/>
+    </row>
+    <row r="1020" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1020" s="72"/>
+    </row>
+    <row r="1021" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1021" s="72"/>
+    </row>
+    <row r="1022" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1022" s="72"/>
+    </row>
+    <row r="1023" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1023" s="72"/>
+    </row>
+    <row r="1024" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1024" s="72"/>
+    </row>
+    <row r="1025" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1025" s="72"/>
+    </row>
+    <row r="1026" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1026" s="72"/>
+    </row>
+    <row r="1027" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1027" s="72"/>
+    </row>
+    <row r="1028" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1028" s="72"/>
+    </row>
+    <row r="1029" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1029" s="72"/>
+    </row>
+    <row r="1030" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1030" s="72"/>
+    </row>
+    <row r="1031" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1031" s="72"/>
+    </row>
+    <row r="1032" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1032" s="72"/>
+    </row>
+    <row r="1033" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1033" s="72"/>
+    </row>
+    <row r="1034" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1034" s="72"/>
+    </row>
+    <row r="1035" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1035" s="72"/>
+    </row>
+    <row r="1036" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1036" s="72"/>
+    </row>
+    <row r="1037" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1037" s="72"/>
+    </row>
+    <row r="1038" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1038" s="72"/>
+    </row>
+    <row r="1039" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1039" s="72"/>
+    </row>
+    <row r="1040" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1040" s="72"/>
+    </row>
+    <row r="1041" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1041" s="72"/>
+    </row>
+    <row r="1042" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1042" s="72"/>
+    </row>
+    <row r="1043" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1043" s="72"/>
+    </row>
+    <row r="1044" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E1044" s="72"/>
+    </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="42">
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="A105:C105"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="A118:C118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="E136:F136"/>
+    <mergeCell ref="A127:C127"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="A128:C128"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="A135:C135"/>
+    <mergeCell ref="E135:F135"/>
+    <mergeCell ref="A92:C92"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="A117:C117"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="E44:F44"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="A68:C68"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="A69:C69"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="E89:F89"/>
-    <mergeCell ref="A90:C90"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="A108:C108"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="A107:C107"/>
-    <mergeCell ref="E107:F107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>